<commit_message>
Added PH  and another data file
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vsc projects python\pushing limits\SMRS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E43DAF9-D015-4A58-BE13-4C0630FBA792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31D794E-84DA-4D58-A548-499C9B8F31FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{C3DAACF2-C652-4207-9549-90353D674DE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37B714F3-BBA5-4E4F-97C2-279D0ED9B5EE}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,6 +490,48 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
+        <v>105</v>
+      </c>
+      <c r="C6" s="2">
+        <v>8.5</v>
+      </c>
+      <c r="D6" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2">
+        <v>105</v>
+      </c>
+      <c r="C7" s="2">
+        <v>9.5</v>
+      </c>
+      <c r="D7" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2">
+        <v>105</v>
+      </c>
+      <c r="C8" s="2">
+        <v>9</v>
+      </c>
+      <c r="D8" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>